<commit_message>
checkstyle rules are added to engine-xxx projects
</commit_message>
<xml_diff>
--- a/calculation-engine/engine-core-demo/src/main/resources/excel/bak/define.xlsx
+++ b/calculation-engine/engine-core-demo/src/main/resources/excel/bak/define.xlsx
@@ -5,16 +5,16 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\work\spreadsheet_analytics\project\calculation-engine\engine-core-demo\src\main\resources\excel\define-funcexec\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\work\spreadsheet_analytics\project\calculation-engine\engine-core-demo\src\main\resources\excel\bak\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="450" windowWidth="28800" windowHeight="12570"/>
+    <workbookView minimized="1" xWindow="0" yWindow="900" windowWidth="28800" windowHeight="12570"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="152511"/>
+  <calcPr calcId="152511" concurrentCalc="0"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -24,33 +24,21 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
-  <si>
-    <t>Input 1</t>
-  </si>
-  <si>
-    <t>Input 2</t>
-  </si>
-  <si>
-    <t>Constant</t>
-  </si>
-  <si>
-    <t>Multiplier</t>
-  </si>
-  <si>
-    <t>Formula</t>
-  </si>
-  <si>
-    <t>Output 1</t>
-  </si>
-  <si>
-    <t>Output 2</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="5">
   <si>
     <t>Define 1</t>
   </si>
   <si>
-    <t>Define 2</t>
+    <t>a</t>
+  </si>
+  <si>
+    <t>b</t>
+  </si>
+  <si>
+    <t>formula</t>
+  </si>
+  <si>
+    <t>c(a)</t>
   </si>
 </sst>
 </file>
@@ -368,10 +356,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G7"/>
+  <dimension ref="A1:D6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H7" sqref="H7"/>
+      <selection activeCell="I11" sqref="I11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -380,64 +368,39 @@
     <col min="4" max="4" width="9.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
+        <v>1</v>
+      </c>
+      <c r="B1" t="s">
+        <v>2</v>
+      </c>
+      <c r="C1" t="s">
+        <v>3</v>
+      </c>
+      <c r="D1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B2">
+        <v>5</v>
+      </c>
+      <c r="C2">
+        <f>A2+B2</f>
+        <v>5</v>
+      </c>
+      <c r="D2">
+        <f>C2</f>
+        <v>5</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" t="s">
-        <v>2</v>
-      </c>
-      <c r="D1" t="s">
-        <v>3</v>
-      </c>
-      <c r="E1" t="s">
-        <v>4</v>
-      </c>
-      <c r="F1" t="s">
-        <v>5</v>
-      </c>
-      <c r="G1" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="C2">
-        <v>14</v>
-      </c>
-      <c r="D2">
-        <v>0.85</v>
-      </c>
-      <c r="E2">
-        <f>A2*COS(B2)/D2+C2</f>
-        <v>14</v>
-      </c>
-      <c r="F2">
-        <f>E2+1</f>
-        <v>15</v>
-      </c>
-      <c r="G2">
-        <f>E2+2</f>
-        <v>16</v>
-      </c>
-    </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
-        <v>7</v>
-      </c>
       <c r="B6" t="e">
-        <f ca="1">DEFINE("DEVDEF_1", A2,B2,"#",F2,G2)</f>
-        <v>#NAME?</v>
-      </c>
-    </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
-        <v>8</v>
-      </c>
-      <c r="B7" t="e">
-        <f ca="1">DEFINE("DEVDEF_2",A2,"#",G2)</f>
+        <f ca="1">DEFINE("c_from_a",A2,"#",D2)</f>
         <v>#NAME?</v>
       </c>
     </row>

</xml_diff>